<commit_message>
added study session documents
</commit_message>
<xml_diff>
--- a/tests/test01/Test01_Notes_and_links.xlsx
+++ b/tests/test01/Test01_Notes_and_links.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="148">
   <si>
     <t>RC2</t>
   </si>
@@ -486,7 +486,10 @@
     <t>L4 Slide 47</t>
   </si>
   <si>
-    <t>L3 Slide 28</t>
+    <t>Inverse Mod</t>
+  </si>
+  <si>
+    <t>L3 Slide 19</t>
   </si>
 </sst>
 </file>
@@ -844,10 +847,10 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,6 +1027,9 @@
       <c r="F8" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="G8" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>66</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>53</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>54</v>
@@ -1623,7 +1629,7 @@
     <hyperlink ref="F20" r:id="rId26" display="L2 Slide 23"/>
     <hyperlink ref="F21" r:id="rId27" display="L2 Slide 23"/>
     <hyperlink ref="F33" r:id="rId28"/>
-    <hyperlink ref="F39" r:id="rId29"/>
+    <hyperlink ref="F39" r:id="rId29" display="L3 Slide 28"/>
     <hyperlink ref="F22" r:id="rId30" display="L2 Slide 23"/>
     <hyperlink ref="F17" r:id="rId31" display="L2 Slide 23"/>
     <hyperlink ref="F55" r:id="rId32" display="L2 Slide 31"/>
@@ -1640,9 +1646,10 @@
     <hyperlink ref="F69" r:id="rId43"/>
     <hyperlink ref="F55:F58" r:id="rId44" display="L3 Slide 32"/>
     <hyperlink ref="F8" r:id="rId45"/>
+    <hyperlink ref="G8" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -2164,15 +2171,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A478DC777839B84AA78BE34820D6106B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2b0b78b229846a0fb540ef9e6a52c1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e77d71de-ed03-4187-81e7-c51d7bba4b52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a685b91e9f3b401c2950534508025d54" ns3:_="">
     <xsd:import namespace="e77d71de-ed03-4187-81e7-c51d7bba4b52"/>
@@ -2344,6 +2342,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2351,14 +2358,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DAA1A3C-67DD-4598-9E7E-62167BBD3C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0034C2E-083F-4678-AC72-7D9E121334AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2376,16 +2375,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DAA1A3C-67DD-4598-9E7E-62167BBD3C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35899522-1E86-4974-B69A-65376177F53F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="e77d71de-ed03-4187-81e7-c51d7bba4b52"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>

</xml_diff>

<commit_message>
added ECDH, updated spreadsheet
</commit_message>
<xml_diff>
--- a/tests/test01/Test01_Notes_and_links.xlsx
+++ b/tests/test01/Test01_Notes_and_links.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="153">
   <si>
     <t>RC2</t>
   </si>
@@ -388,9 +388,6 @@
     <t>L3 Slide 16</t>
   </si>
   <si>
-    <t>Password + Salt + desired key Len</t>
-  </si>
-  <si>
     <t>L3 Slide 17</t>
   </si>
   <si>
@@ -490,6 +487,25 @@
   </si>
   <si>
     <t>L3 Slide 19</t>
+  </si>
+  <si>
+    <t>Pick G (cyclic group)</t>
+  </si>
+  <si>
+    <t>Block Padding</t>
+  </si>
+  <si>
+    <t>KDF</t>
+  </si>
+  <si>
+    <t>Key Derivation Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password + Salt + desired key Len
+</t>
+  </si>
+  <si>
+    <t>key derivation function (KDF) is a cryptographic hash function that derives one or more secret keys from a secret value such as a master key, a password, or a passphrase using a pseudorandom function.[1][2] KDFs can be used to stretch keys into longer keys or to obtain keys of a required format, such as converting a group element that is the result of a Diffie–Hellman key exchange into a symmetric key for use with AES</t>
   </si>
 </sst>
 </file>
@@ -844,13 +860,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,13 +1038,13 @@
         <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>66</v>
@@ -1069,15 +1085,17 @@
         <v>52</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1090,7 +1108,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H12" s="4"/>
     </row>
@@ -1141,13 +1159,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>80</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H17" s="4"/>
     </row>
@@ -1204,13 +1222,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="F22" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="H22" s="4"/>
     </row>
@@ -1226,7 +1244,7 @@
         <v>47</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H25" s="4"/>
     </row>
@@ -1235,10 +1253,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H26" s="4"/>
     </row>
@@ -1247,10 +1268,13 @@
         <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H27" s="4"/>
     </row>
@@ -1259,10 +1283,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H28" s="4"/>
     </row>
@@ -1271,10 +1298,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H29" s="4"/>
     </row>
@@ -1283,10 +1313,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H30" s="4"/>
     </row>
@@ -1295,332 +1328,354 @@
         <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F32" s="4"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>116</v>
+        <v>50</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H39" s="4" t="s">
+      <c r="F42" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H42" s="4"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H43" s="4"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H45" s="4"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" ht="186" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="1:8" ht="186" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E52" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F53" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F54" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F55" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="4" t="s">
+      <c r="E56" s="5"/>
+      <c r="F56" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E54" s="5"/>
-      <c r="F54" s="4"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F56" s="4"/>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>74</v>
-      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="4"/>
+      <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F59" s="4"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H60" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H61" s="4"/>
+      <c r="E63" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>133</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H64" s="4"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G70" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G67" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F72" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F69" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>135</v>
+      <c r="G72" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F35" r:id="rId1"/>
+    <hyperlink ref="F33" r:id="rId1"/>
     <hyperlink ref="F2" r:id="rId2"/>
     <hyperlink ref="F6" r:id="rId3"/>
     <hyperlink ref="F5" r:id="rId4"/>
     <hyperlink ref="F7" r:id="rId5"/>
     <hyperlink ref="H8" r:id="rId6"/>
-    <hyperlink ref="G33" r:id="rId7"/>
-    <hyperlink ref="H48" r:id="rId8"/>
+    <hyperlink ref="G36" r:id="rId7"/>
+    <hyperlink ref="H51" r:id="rId8"/>
     <hyperlink ref="H6" r:id="rId9"/>
-    <hyperlink ref="H9:H38" r:id="rId10" display="."/>
-    <hyperlink ref="H39" r:id="rId11"/>
-    <hyperlink ref="H57" r:id="rId12"/>
-    <hyperlink ref="H33" r:id="rId13" display="python DH.py"/>
-    <hyperlink ref="F37" r:id="rId14" display="L2 Slide 41"/>
-    <hyperlink ref="F48" r:id="rId15" display="L2 Slide 41"/>
-    <hyperlink ref="F50" r:id="rId16" display="L2 Slide 41"/>
-    <hyperlink ref="F49" r:id="rId17" display="L2 Slide 41"/>
-    <hyperlink ref="F51" r:id="rId18" display="L2 Slide 41"/>
-    <hyperlink ref="F52" r:id="rId19" display="L2 Slide 41"/>
-    <hyperlink ref="F53" r:id="rId20" display="L2 Slide 41"/>
+    <hyperlink ref="H9:H41" r:id="rId10" display="."/>
+    <hyperlink ref="H42" r:id="rId11"/>
+    <hyperlink ref="H60" r:id="rId12"/>
+    <hyperlink ref="H36" r:id="rId13" display="python DH.py"/>
+    <hyperlink ref="F40" r:id="rId14" display="L2 Slide 41"/>
+    <hyperlink ref="F51" r:id="rId15" display="L2 Slide 41"/>
+    <hyperlink ref="F53" r:id="rId16" display="L2 Slide 41"/>
+    <hyperlink ref="F52" r:id="rId17" display="L2 Slide 41"/>
+    <hyperlink ref="F54" r:id="rId18" display="L2 Slide 41"/>
+    <hyperlink ref="F55" r:id="rId19" display="L2 Slide 41"/>
+    <hyperlink ref="F56" r:id="rId20" display="L2 Slide 41"/>
     <hyperlink ref="F14" r:id="rId21" display="L2 Slide 23"/>
     <hyperlink ref="F15" r:id="rId22" display="L2 Slide 23"/>
     <hyperlink ref="F16" r:id="rId23" display="L2 Slide 23"/>
@@ -1628,23 +1683,23 @@
     <hyperlink ref="F18" r:id="rId25" display="L2 Slide 23"/>
     <hyperlink ref="F20" r:id="rId26" display="L2 Slide 23"/>
     <hyperlink ref="F21" r:id="rId27" display="L2 Slide 23"/>
-    <hyperlink ref="F33" r:id="rId28"/>
-    <hyperlink ref="F39" r:id="rId29" display="L3 Slide 28"/>
+    <hyperlink ref="F36" r:id="rId28"/>
+    <hyperlink ref="F42" r:id="rId29" display="L3 Slide 28"/>
     <hyperlink ref="F22" r:id="rId30" display="L2 Slide 23"/>
     <hyperlink ref="F17" r:id="rId31" display="L2 Slide 23"/>
-    <hyperlink ref="F55" r:id="rId32" display="L2 Slide 31"/>
-    <hyperlink ref="F57" r:id="rId33"/>
-    <hyperlink ref="F58" r:id="rId34" display="L2 Slide 31"/>
-    <hyperlink ref="F64" r:id="rId35" display="L2 Slide 31"/>
-    <hyperlink ref="G64" r:id="rId36" display="conversion_table.pdf"/>
-    <hyperlink ref="G67" r:id="rId37"/>
+    <hyperlink ref="F58" r:id="rId32" display="L2 Slide 31"/>
+    <hyperlink ref="F60" r:id="rId33"/>
+    <hyperlink ref="F61" r:id="rId34" display="L2 Slide 31"/>
+    <hyperlink ref="F67" r:id="rId35" display="L2 Slide 31"/>
+    <hyperlink ref="G67" r:id="rId36" display="conversion_table.pdf"/>
+    <hyperlink ref="G70" r:id="rId37"/>
     <hyperlink ref="F25:F31" r:id="rId38" display="L2 Slide 23"/>
     <hyperlink ref="G11" r:id="rId39" display="https://asecuritysite.com/encryption/elgamal"/>
-    <hyperlink ref="G69" r:id="rId40"/>
+    <hyperlink ref="G72" r:id="rId40"/>
     <hyperlink ref="F11" r:id="rId41"/>
     <hyperlink ref="F12" r:id="rId42"/>
-    <hyperlink ref="F69" r:id="rId43"/>
-    <hyperlink ref="F55:F58" r:id="rId44" display="L3 Slide 32"/>
+    <hyperlink ref="F72" r:id="rId43"/>
+    <hyperlink ref="F58:F61" r:id="rId44" display="L3 Slide 32"/>
     <hyperlink ref="F8" r:id="rId45"/>
     <hyperlink ref="G8" r:id="rId46"/>
   </hyperlinks>
@@ -2171,6 +2226,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A478DC777839B84AA78BE34820D6106B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2b0b78b229846a0fb540ef9e6a52c1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e77d71de-ed03-4187-81e7-c51d7bba4b52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a685b91e9f3b401c2950534508025d54" ns3:_="">
     <xsd:import namespace="e77d71de-ed03-4187-81e7-c51d7bba4b52"/>
@@ -2342,15 +2406,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2358,6 +2413,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DAA1A3C-67DD-4598-9E7E-62167BBD3C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0034C2E-083F-4678-AC72-7D9E121334AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2371,14 +2434,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DAA1A3C-67DD-4598-9E7E-62167BBD3C8A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>